<commit_message>
funksjon for database utskrift i commit
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -476,15 +476,11 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>34323434</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12345678921</t>
-        </is>
+      <c r="E2" t="n">
+        <v>34323434</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12345678921</v>
       </c>
     </row>
     <row r="3">
@@ -504,15 +500,11 @@
           <t>Norge</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>23334343</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>12345678922</t>
-        </is>
+      <c r="E3" t="n">
+        <v>23334343</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12345678922</v>
       </c>
     </row>
     <row r="4">
@@ -532,15 +524,11 @@
           <t>Kristiansand</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>22233666</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>12345678901</t>
-        </is>
+      <c r="E4" t="n">
+        <v>22233666</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12345678901</v>
       </c>
     </row>
     <row r="5">
@@ -560,15 +548,11 @@
           <t>Kristiansand</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>22233666</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>12345678901</t>
-        </is>
+      <c r="E5" t="n">
+        <v>22233666</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12345678901</v>
       </c>
     </row>
   </sheetData>
@@ -783,10 +767,8 @@
       <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>12345678911</t>
-        </is>
+      <c r="C2" t="n">
+        <v>12345678911</v>
       </c>
     </row>
     <row r="3">
@@ -796,10 +778,8 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>12345678901</t>
-        </is>
+      <c r="C3" t="n">
+        <v>12345678901</v>
       </c>
     </row>
   </sheetData>
@@ -914,10 +894,8 @@
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="M2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -959,10 +937,8 @@
           <t>2024-11-21</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>2121323</t>
-        </is>
+      <c r="M3" t="n">
+        <v>2121323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fixes, removed unused imports
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -470,10 +470,22 @@
       <c r="B2" t="n">
         <v>6</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>knsjndkfnj</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nfknkfndk</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>232121232</v>
+      </c>
+      <c r="F2" t="n">
+        <v>434345</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -482,10 +494,22 @@
       <c r="B3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>snnsjfndjs</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nkfnkfndk</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>122232</v>
+      </c>
+      <c r="F3" t="n">
+        <v>121213342</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -496,15 +520,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jill</t>
+          <t>Schlorpt</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>34323434</v>
+        <v>8374363</v>
       </c>
       <c r="F4" t="n">
-        <v>12345678921</v>
+        <v>12345678901</v>
       </c>
     </row>
     <row r="5">
@@ -516,19 +540,19 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Glorpo</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Norge</t>
+          <t>Tilted Towers</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>23334343</v>
+        <v>75757</v>
       </c>
       <c r="F5" t="n">
-        <v>12345678922</v>
+        <v>100922846373</v>
       </c>
     </row>
     <row r="6">
@@ -540,19 +564,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Kristin Norge</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Kristiansand</t>
-        </is>
-      </c>
+          <t>Schlorpt</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>22233666</v>
+        <v>757574</v>
       </c>
       <c r="F6" t="n">
-        <v>12345678901</v>
+        <v>230323434543</v>
       </c>
     </row>
     <row r="7">
@@ -564,19 +584,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jon Norge</t>
+          <t>Glorpo</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kristiansand</t>
+          <t>Tilted Towers</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>22233666</v>
+        <v>9865463</v>
       </c>
       <c r="F7" t="n">
-        <v>12345678901</v>
+        <v>100922846373</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +811,9 @@
       <c r="B2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>343434</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -801,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>12345678911</v>
+        <v>10070467433</v>
       </c>
     </row>
     <row r="4">
@@ -812,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>12345678901</v>
+        <v>10070467433</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -924,7 +946,7 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>2121</v>
+        <v>23232</v>
       </c>
     </row>
     <row r="3">
@@ -945,21 +967,17 @@
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2,5,3</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>21232</v>
       </c>
     </row>
     <row r="4">
@@ -979,30 +997,18 @@
         <v>1</v>
       </c>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>on</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>2024-11-21</t>
-        </is>
-      </c>
+          <t>1,3,4,5</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
-        <v>2121323</v>
+        <v>736372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>